<commit_message>
Cron_job functions updated (custom province)
</commit_message>
<xml_diff>
--- a/CANDEV2020 Energy Loads.xlsx
+++ b/CANDEV2020 Energy Loads.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alberta" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -54,12 +56,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,13 +341,14 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11.5703125" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="6" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -352,7 +357,7 @@
           <t xml:space="preserve">Date </t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Hour </t>
         </is>
@@ -369,7 +374,7 @@
           <t>18-Jan-2020</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>23:03</t>
         </is>
@@ -386,7 +391,7 @@
           <t>18-Jan-2020</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>23:13</t>
         </is>
@@ -403,7 +408,7 @@
           <t>18-Jan-2020</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>23:17</t>
         </is>
@@ -420,7 +425,7 @@
           <t>19-Jan-2020</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>06:30</t>
         </is>
@@ -437,7 +442,7 @@
           <t>19-Jan-2020</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>06:31</t>
         </is>
@@ -454,7 +459,7 @@
           <t>19-Jan-2020</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>06:32</t>
         </is>
@@ -462,6 +467,295 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>10267</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>07:09</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10424</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10426</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10426</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>07:14</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10424</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>07:19</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10440</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>07:22</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10415</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>10420</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>07:23</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>10420</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>07:24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10425</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>10449</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>07:27</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>10449</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10454</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10444</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>07:34</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10451</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>07:34</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10451</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10450</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>10450</t>
         </is>
       </c>
     </row>
@@ -480,13 +774,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.140625" customWidth="1" style="6" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -494,7 +791,7 @@
           <t xml:space="preserve">Date </t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Hour </t>
         </is>
@@ -508,136 +805,361 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24:00</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>18206</v>
+        <v>16547</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18206</v>
+        <v>16173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18206</v>
+        <v>16027</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18206</v>
+        <v>15912</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>18206</v>
+        <v>16023</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18206</v>
+        <v>16091</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18206</v>
+        <v>16268</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>18206</v>
+        <v>16439</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18206</v>
+        <v>16536</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>16855</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>17266</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>17451</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>17692</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>17699</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>17711</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>9:00</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>17187</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>17667</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>18553</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>18519</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>5:00</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>18298</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>4:00</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>18238</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>3:00</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>18561</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2:00</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>17992</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2020-01-17</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>17121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrape NB (not working corrupts excel)
</commit_message>
<xml_diff>
--- a/CANDEV2020 Energy Loads.xlsx
+++ b/CANDEV2020 Energy Loads.xlsx
@@ -1,76 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alberta" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ontario" sheetId="2" state="visible" r:id="rId2"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
-</workbook>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="2">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-</styleSheet>
-</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -339,428 +266,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="6" min="2" max="2"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Date </t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hour </t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hour</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Load (MW)</t>
+          <t>Load(MW)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>23:03</t>
+          <t>19-Jan-2020</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10562</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>18-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>23:13</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10584</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>18-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>23:17</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>10577</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>06:30</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>10254</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>06:31</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>10259</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>06:32</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10267</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B8" s="6" t="inlineStr">
-        <is>
-          <t>07:09</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>10424</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B9" s="6" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>10426</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B10" s="6" t="inlineStr">
-        <is>
-          <t>07:11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>10426</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B11" s="6" t="inlineStr">
-        <is>
-          <t>07:14</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>10424</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B12" s="6" t="inlineStr">
-        <is>
-          <t>07:19</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>10440</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B13" s="6" t="inlineStr">
-        <is>
-          <t>07:22</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>10415</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B14" s="6" t="inlineStr">
-        <is>
-          <t>07:23</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>10420</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B15" s="6" t="inlineStr">
-        <is>
-          <t>07:23</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>10420</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B16" s="6" t="inlineStr">
-        <is>
-          <t>07:24</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>10425</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B17" s="6" t="inlineStr">
-        <is>
-          <t>07:27</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>10449</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B18" s="6" t="inlineStr">
-        <is>
-          <t>07:27</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>10449</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B19" s="6" t="inlineStr">
-        <is>
-          <t>07:29</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>10454</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B20" s="6" t="inlineStr">
-        <is>
-          <t>07:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>10444</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>07:34</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>10451</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>07:34</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>10451</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>07:35</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>10450</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>19-Jan-2020</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>07:35</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>10450</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
+          <t>10731</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -776,34 +322,31 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9.140625" customWidth="1" style="6" min="2" max="2"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Date </t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hour </t>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hour</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Load (MW)</t>
+          <t>Load(MW)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2020-01-17</t>
         </is>

</xml_diff>